<commit_message>
Fixing working tree, pushing a bunch of SubBoards and FlatPack BOM
</commit_message>
<xml_diff>
--- a/Bill of Materials/FusIon Pack.xlsx
+++ b/Bill of Materials/FusIon Pack.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7656"/>
   </bookViews>
   <sheets>
     <sheet name="Fusion Pack Rev 0-1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <definedName name="FusIon_Pack" localSheetId="0">'Fusion Pack Rev 0-1'!$A$1:$K$51</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1757,25 +1758,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="61.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="52.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.44140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="115" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1807,7 +1808,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
@@ -1834,7 +1835,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>41</v>
       </c>
@@ -1861,7 +1862,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
@@ -1888,7 +1889,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>111</v>
       </c>
@@ -1912,7 +1913,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>100</v>
       </c>
@@ -1945,7 +1946,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>103</v>
       </c>
@@ -1978,7 +1979,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="18" t="s">
         <v>106</v>
       </c>
@@ -2011,7 +2012,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30" t="s">
         <v>89</v>
       </c>
@@ -2044,7 +2045,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" s="20" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
         <v>107</v>
       </c>
@@ -2077,7 +2078,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" s="20" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>110</v>
       </c>
@@ -2110,7 +2111,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="30" t="s">
         <v>114</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>119</v>
       </c>
@@ -2176,7 +2177,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>121</v>
       </c>
@@ -2209,7 +2210,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>95</v>
       </c>
@@ -2242,7 +2243,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>64</v>
       </c>
@@ -2275,7 +2276,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>88</v>
       </c>
@@ -2308,7 +2309,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>67</v>
       </c>
@@ -2341,7 +2342,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>70</v>
       </c>
@@ -2374,7 +2375,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="36" t="s">
         <v>25</v>
       </c>
@@ -2407,7 +2408,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>74</v>
       </c>
@@ -2440,7 +2441,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="38" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="36" t="s">
         <v>73</v>
       </c>
@@ -2473,7 +2474,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>132</v>
       </c>
@@ -2506,7 +2507,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>77</v>
       </c>
@@ -2539,7 +2540,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>137</v>
       </c>
@@ -2572,7 +2573,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" s="32" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30" t="s">
         <v>46</v>
       </c>
@@ -2605,7 +2606,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>169</v>
       </c>
@@ -2638,7 +2639,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="24" t="s">
         <v>143</v>
       </c>
@@ -2671,7 +2672,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>164</v>
       </c>
@@ -2704,7 +2705,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
         <v>154</v>
       </c>
@@ -2737,7 +2738,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>150</v>
       </c>
@@ -2770,7 +2771,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>155</v>
       </c>
@@ -2803,7 +2804,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>172</v>
       </c>
@@ -2836,7 +2837,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>168</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
         <v>48</v>
       </c>
@@ -2902,7 +2903,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" s="26" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
         <v>98</v>
       </c>
@@ -2935,7 +2936,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="24" t="s">
         <v>53</v>
       </c>
@@ -2968,7 +2969,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>71</v>
       </c>
@@ -3001,7 +3002,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
         <v>57</v>
       </c>
@@ -3034,7 +3035,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
         <v>60</v>
       </c>
@@ -3067,7 +3068,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" s="14" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>27</v>
       </c>
@@ -3100,7 +3101,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
         <v>23</v>
       </c>
@@ -3133,7 +3134,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="24" t="s">
         <v>96</v>
       </c>
@@ -3166,7 +3167,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="24" t="s">
         <v>135</v>
       </c>
@@ -3199,7 +3200,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="24" t="s">
         <v>203</v>
       </c>
@@ -3232,7 +3233,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="24" t="s">
         <v>90</v>
       </c>
@@ -3265,7 +3266,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12" t="s">
         <v>51</v>
       </c>
@@ -3298,7 +3299,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12" t="s">
         <v>62</v>
       </c>
@@ -3331,7 +3332,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="24" t="s">
         <v>55</v>
       </c>
@@ -3364,7 +3365,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12" t="s">
         <v>7</v>
       </c>
@@ -3397,7 +3398,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="24" t="s">
         <v>183</v>
       </c>
@@ -3430,7 +3431,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D53" s="7" t="s">
         <v>256</v>
       </c>
@@ -3439,7 +3440,7 @@
         <v>166.79699989999995</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D54" s="4" t="s">
         <v>257</v>
       </c>

</xml_diff>